<commit_message>
Se terminan de atender las observaciones en Comisiones Legislativas
</commit_message>
<xml_diff>
--- a/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
+++ b/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Programacion_FJMD\#C\01_App_PLE_INEGI\A_Retroalimentaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A747F85-605E-4CBB-997D-F2D51E80FEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA21085-56C7-4865-AC47-259F6273802E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>Hoja</t>
   </si>
@@ -616,27 +616,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1016,10 +996,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1332,7 +1312,9 @@
       <c r="D13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="19"/>
+      <c r="E13" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="12"/>
@@ -1352,7 +1334,9 @@
       <c r="D14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="10"/>
@@ -1370,12 +1354,16 @@
       <c r="D15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="L15" s="16"/>
     </row>
@@ -1390,7 +1378,9 @@
       <c r="D16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="10"/>
@@ -1408,7 +1398,9 @@
       <c r="D17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
       <c r="L17" s="16"/>
@@ -2110,10 +2102,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E3:E17">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Se estan agregando nuevas validaciones en Personas Legisladoras
</commit_message>
<xml_diff>
--- a/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
+++ b/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Programacion_FJMD\#C\01_App_PLE_INEGI\A_Retroalimentaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA21085-56C7-4865-AC47-259F6273802E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6559390-B58A-40C5-B27B-2BFE6A029D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="105">
   <si>
     <t>Hoja</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>Se agrega validación adicional de no permitir entrada manual de fecha</t>
+  </si>
+  <si>
+    <t>Esto se debe a los procesos internos del aplicativo, se optimizará al final del proyecto.</t>
+  </si>
+  <si>
+    <t>falta guardado</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1002,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:A17"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1418,7 +1424,7 @@
       <c r="D18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="19"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="13"/>
@@ -1439,7 +1445,9 @@
         <v>78</v>
       </c>
       <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="F19" s="18" t="s">
+        <v>103</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="L19" s="16"/>
     </row>
@@ -1454,7 +1462,9 @@
       <c r="D20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="L20" s="16"/>
@@ -1470,7 +1480,9 @@
       <c r="D21" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
         <v>63</v>
@@ -1488,7 +1500,9 @@
       <c r="D22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
         <v>83</v>
@@ -1506,7 +1520,9 @@
       <c r="D23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="L23" s="16"/>
@@ -1522,7 +1538,9 @@
       <c r="D24" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="L24" s="16"/>
@@ -1538,7 +1556,9 @@
       <c r="D25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="L25" s="16"/>
@@ -1554,7 +1574,9 @@
       <c r="D26" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="L26" s="16"/>
@@ -1570,7 +1592,9 @@
       <c r="D27" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="L27" s="16"/>
@@ -1586,7 +1610,9 @@
       <c r="D28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18" t="s">
         <v>84</v>
@@ -1604,7 +1630,9 @@
       <c r="D29" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
         <v>85</v>
@@ -1622,7 +1650,9 @@
       <c r="D30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="L30" s="16"/>
@@ -1639,7 +1669,9 @@
         <v>35</v>
       </c>
       <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="F31" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="G31" s="18" t="s">
         <v>67</v>
       </c>
@@ -1657,7 +1689,9 @@
         <v>35</v>
       </c>
       <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="F32" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="G32" s="18"/>
       <c r="L32" s="16"/>
     </row>
@@ -2101,7 +2135,7 @@
     <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E3:E17">
+  <conditionalFormatting sqref="E3:E57">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
@@ -2115,7 +2149,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H16 E3:E17" xr:uid="{32FA0E09-31A7-48C0-A844-3C55608E19D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H16 E3:E57" xr:uid="{32FA0E09-31A7-48C0-A844-3C55608E19D8}">
       <formula1>"Pendiente, Completa"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Se limpia codigo de escolaridad
</commit_message>
<xml_diff>
--- a/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
+++ b/A_Retroalimentaciones/Formato_retro_PLE (01Agosto2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Programacion_FJMD\#C\01_App_PLE_INEGI\A_Retroalimentaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6559390-B58A-40C5-B27B-2BFE6A029D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C553A93C-D417-4C26-B1A3-8FF54B1831AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>Hoja</t>
   </si>
@@ -1002,10 +1002,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1722,9 @@
       <c r="D34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="18"/>
+      <c r="E34" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="L34" s="16"/>
@@ -1738,7 +1740,9 @@
       <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="L35" s="16"/>

</xml_diff>